<commit_message>
readme update and rename the figure analysis plot
</commit_message>
<xml_diff>
--- a/Application/Input/parameter_input.xlsx
+++ b/Application/Input/parameter_input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaomiyang/Documents/GitHub/SubmittedActiveSamplingforTechnometrics/ActiveSampling/Application/Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaomiyang/Documents/GitHub/Check reproducibility/ActiveSampling/Application/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DA1111-B652-8641-A688-8EBA86A7AFAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5127F3-9348-4E4D-863B-01CE5FE07BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,7 +391,7 @@
   <dimension ref="A1:AMK3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -419,13 +419,13 @@
     </row>
     <row r="2" spans="1:5" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>10</v>
+        <v>500</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="D2"/>
       <c r="E2"/>

</xml_diff>